<commit_message>
recreated all kaycee's card to have borders
</commit_message>
<xml_diff>
--- a/Répartition.xlsx
+++ b/Répartition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\-FR-InscryptionPrintableCards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\Repo Bordel\-FR-InscryptionPrintableCards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA86C9B-6E04-4CCA-B3DA-22205DDDCC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4E6952-F102-4F0F-A4B5-99720AA43D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>Vipere</t>
   </si>
@@ -388,9 +388,6 @@
     <t>Scara-bouffe</t>
   </si>
   <si>
-    <t>Tortue boueuse</t>
-  </si>
-  <si>
     <t>Louveteau sinistre</t>
   </si>
   <si>
@@ -415,10 +412,25 @@
     <t>ouroboros écriture corrigée (nerf bone)</t>
   </si>
   <si>
-    <t>regarder autre token</t>
-  </si>
-  <si>
     <t>buff du ring worm</t>
+  </si>
+  <si>
+    <t>nerf direworl/pup</t>
+  </si>
+  <si>
+    <t>nerf grizzly</t>
+  </si>
+  <si>
+    <t>nerf homme papillon</t>
+  </si>
+  <si>
+    <t>Tortue palustre</t>
+  </si>
+  <si>
+    <t>regarder autre token (evolutions)</t>
+  </si>
+  <si>
+    <t>L'ancêtre</t>
   </si>
 </sst>
 </file>
@@ -746,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1011,7 @@
         <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -1032,7 +1044,7 @@
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1117,7 +1129,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G33" t="s">
         <v>99</v>
@@ -1197,7 +1209,7 @@
         <v>115</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,7 +1217,7 @@
         <v>6</v>
       </c>
       <c r="I47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -1213,7 +1225,7 @@
         <v>59</v>
       </c>
       <c r="I48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1221,7 +1233,7 @@
         <v>12</v>
       </c>
       <c r="I49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -1229,7 +1241,7 @@
         <v>116</v>
       </c>
       <c r="I50" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -1237,7 +1249,7 @@
         <v>60</v>
       </c>
       <c r="I51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -1247,20 +1259,29 @@
       <c r="B52">
         <v>0</v>
       </c>
+      <c r="I52" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
+      <c r="I53" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="I54" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -1286,6 +1307,11 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ossifrage and broken egg
</commit_message>
<xml_diff>
--- a/Répartition.xlsx
+++ b/Répartition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Documents\Repo Bordel\-FR-InscryptionPrintableCards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\-FR-InscryptionPrintableCards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C027F23-EB91-4071-92AE-969684D5E6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A117637A-2DA0-4E88-8896-5BE7FCFF35E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Vipere</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Reine des fourmies</t>
   </si>
   <si>
-    <t>Terrain/Non Vivant</t>
-  </si>
-  <si>
     <t>Seau à Appats</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
     <t>Fourmi guerrière</t>
   </si>
   <si>
-    <t>Loup sinistre (token)</t>
-  </si>
-  <si>
     <t>Mite gloutonne</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
     <t>Louveteau sinistre</t>
   </si>
   <si>
-    <t>Tortue boueuse (token)</t>
-  </si>
-  <si>
     <t>Tétard</t>
   </si>
   <si>
@@ -427,9 +418,6 @@
     <t>L'ancêtre</t>
   </si>
   <si>
-    <t>Vautour barbu</t>
-  </si>
-  <si>
     <t>Objets</t>
   </si>
   <si>
@@ -464,6 +452,30 @@
   </si>
   <si>
     <t>Loup en cage</t>
+  </si>
+  <si>
+    <t>Ossifrage</t>
+  </si>
+  <si>
+    <t>Wapiti (token)</t>
+  </si>
+  <si>
+    <t>L'ancêtre (token)</t>
+  </si>
+  <si>
+    <t>Loup (token)</t>
+  </si>
+  <si>
+    <t>Fourmi (token)</t>
+  </si>
+  <si>
+    <t>Tortue palustre (token)</t>
+  </si>
+  <si>
+    <t>nerf Grand requin blanc</t>
+  </si>
+  <si>
+    <t>Coquille œuf</t>
   </si>
 </sst>
 </file>
@@ -791,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,10 +817,11 @@
     <col min="4" max="4" width="5.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="3.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.28515625" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -817,7 +830,7 @@
       </c>
       <c r="B1">
         <f>SUM(B2:B63)</f>
-        <v>0</v>
+        <v>191</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -827,29 +840,30 @@
         <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1">
-        <f>SUM(H2:H18)</f>
-        <v>0</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F1">
+        <f>SUM(F2:F25)</f>
+        <v>67</v>
+      </c>
+      <c r="G1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J1">
         <f>SUM(J2:J11)</f>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -858,107 +872,143 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>146</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>103</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J6">
         <v>3</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -967,96 +1017,129 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J7">
         <v>3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" t="s">
-        <v>75</v>
+        <v>143</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J8">
         <v>6</v>
       </c>
+      <c r="M8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J9">
         <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J10">
         <v>3</v>
+      </c>
+      <c r="M10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" t="s">
-        <v>31</v>
+        <v>115</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J11">
         <v>3</v>
@@ -1064,428 +1147,580 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>107</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J12">
         <v>3</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="I13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
         <v>55</v>
       </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" t="s">
-        <v>88</v>
-      </c>
-      <c r="J14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" t="s">
-        <v>56</v>
-      </c>
       <c r="J15">
         <v>2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>108</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
       </c>
       <c r="E17" t="s">
         <v>110</v>
       </c>
-      <c r="G17" t="s">
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="M17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>91</v>
+      </c>
+      <c r="I29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="G30" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>93</v>
+      </c>
+      <c r="I31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>86</v>
       </c>
-      <c r="G29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>89</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="G32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" t="s">
-        <v>95</v>
+      <c r="I32" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>113</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="I33" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="I34" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="I35" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>65</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="I37" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>104</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>47</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>51</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>111</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>113</v>
-      </c>
-      <c r="I47" t="s">
-        <v>120</v>
+        <v>11</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>6</v>
-      </c>
-      <c r="I48" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>57</v>
       </c>
-      <c r="I49" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I50" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>114</v>
       </c>
-      <c r="I51" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
-      </c>
-      <c r="I52" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>0</v>
       </c>
-      <c r="I53" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="I54" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>85</v>
+        <v>25</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B61">
-    <sortCondition ref="A61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:D15">
+    <sortCondition ref="C2:C15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>